<commit_message>
modified excel and learn ddt
</commit_message>
<xml_diff>
--- a/testFile/case/user.xlsx
+++ b/testFile/case/user.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="testlearn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,64 +31,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>case_name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>method</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>login</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>paramData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>isExec</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录</t>
+    <rPh sb="0" eb="1">
+      <t>deng lu</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户正常登录</t>
+    <rPh sb="1" eb="2">
+      <t>zheng chang</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>deng lu</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户密码错误</t>
+    <rPh sb="0" eb="1">
+      <t>yong hu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>mi ma</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>cuo wu</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/test/api/user/doLogin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>post</t>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mobilePhone</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>validateCode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>success</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>message</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>null</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>18408249437</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>999999</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>200</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "name":"uu",
+    "password":"123455"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+{
+    "name":"1",
+    "password":"111111"
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruleResData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>expectedResData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": 200,
+    "message": "success",
+    "data": "登录成功"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": 4001,
+    "message": "faild",
+    "data": "用户名或密码错误"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>trueResDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -159,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -170,6 +258,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,75 +548,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="2"/>
-    <col min="8" max="8" width="46" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="14" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="20.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="107" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -527,4 +677,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add testcase and check datas
</commit_message>
<xml_diff>
--- a/testFile/case/user.xlsx
+++ b/testFile/case/user.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>token</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -131,10 +131,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ruleResData</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>expectedResData</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -155,27 +151,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>result</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code": 200}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code": 4001}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruleResData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>trueResDate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>result</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
+    <t>{"code": 200,"message":"sucess"}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -550,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -565,20 +577,20 @@
     <col min="7" max="7" width="17.6640625" style="2" customWidth="1"/>
     <col min="8" max="9" width="20.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" style="2" customWidth="1"/>
     <col min="13" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -596,16 +608,16 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="120" x14ac:dyDescent="0.2">
@@ -634,10 +646,10 @@
         <v>17</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="107" customHeight="1" x14ac:dyDescent="0.2">
@@ -666,10 +678,10 @@
         <v>16</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -681,29 +693,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -713,8 +729,11 @@
       <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -723,6 +742,9 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add write excel method
</commit_message>
<xml_diff>
--- a/testFile/case/user.xlsx
+++ b/testFile/case/user.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangqian/Documents/python-request/testFile/case/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="1"/>
   </bookViews>
@@ -18,20 +13,20 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>token</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -190,11 +185,19 @@
     <t>{"code": 200,"message":"sucess"}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -255,11 +258,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -279,6 +293,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +586,7 @@
       <selection activeCell="J1" sqref="J1:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
@@ -582,7 +602,7 @@
     <col min="13" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -620,7 +640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="112" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -652,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="107" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="107" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -693,19 +713,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="32.5" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -718,10 +738,13 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -733,14 +756,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="7" t="s">

</xml_diff>